<commit_message>
fix 28.10.2024 price 13.5
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/templates/templateRDT-B.xlsx
+++ b/TeplosilaWeb/Content/templates/templateRDT-B.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Документы\Рабочая папка\ТЗ программа подбора TRV, RDT\templates\Новые RDT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pge27\OneDrive\Рабочий стол\TeploSilaWeb\TeplosilaWeb\Content\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCA21F5-F646-4340-BFDE-5697AB1BE288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14220" windowHeight="11265"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -200,7 +201,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -422,6 +423,48 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -443,9 +486,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -454,45 +494,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -828,24 +829,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8" style="3" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" style="3" customWidth="1"/>
-    <col min="8" max="9" width="9.85546875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8" style="3" customWidth="1"/>
+    <col min="6" max="7" width="8.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" style="3" customWidth="1"/>
     <col min="11" max="11" width="8.5703125" style="3" customWidth="1"/>
     <col min="12" max="23" width="9.140625" style="2"/>
   </cols>
@@ -859,12 +860,12 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="18"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -879,19 +880,19 @@
       <c r="W2" s="2"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -906,19 +907,19 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="22"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="36"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -933,19 +934,19 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="26"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="39"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -985,12 +986,12 @@
       <c r="W6" s="2"/>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1012,19 +1013,19 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1039,19 +1040,19 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1066,18 +1067,18 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
       <c r="K10" s="15"/>
       <c r="L10" s="2"/>
       <c r="M10" s="4"/>
@@ -1093,19 +1094,19 @@
       <c r="W10" s="4"/>
     </row>
     <row r="11" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
       <c r="L11" s="2"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
@@ -1120,18 +1121,18 @@
       <c r="W11" s="4"/>
     </row>
     <row r="12" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
       <c r="K12" s="15"/>
       <c r="L12" s="2"/>
       <c r="M12" s="4"/>
@@ -1147,18 +1148,18 @@
       <c r="W12" s="4"/>
     </row>
     <row r="13" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
       <c r="K13" s="15" t="s">
         <v>10</v>
       </c>
@@ -1176,19 +1177,19 @@
       <c r="W13" s="4"/>
     </row>
     <row r="14" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
       <c r="L14" s="2"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
@@ -1203,18 +1204,18 @@
       <c r="W14" s="4"/>
     </row>
     <row r="15" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
       <c r="K15" s="15" t="s">
         <v>10</v>
       </c>
@@ -1232,18 +1233,18 @@
       <c r="W15" s="4"/>
     </row>
     <row r="16" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
       <c r="K16" s="15" t="s">
         <v>10</v>
       </c>
@@ -1261,18 +1262,18 @@
       <c r="W16" s="4"/>
     </row>
     <row r="17" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
       <c r="K17" s="15"/>
       <c r="L17" s="2"/>
       <c r="M17" s="4"/>
@@ -1288,18 +1289,18 @@
       <c r="W17" s="4"/>
     </row>
     <row r="18" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
       <c r="K18" s="15"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
@@ -1340,12 +1341,12 @@
       <c r="W19" s="2"/>
     </row>
     <row r="20" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1367,19 +1368,19 @@
       <c r="W20" s="2"/>
     </row>
     <row r="21" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -1394,19 +1395,19 @@
       <c r="W21" s="2"/>
     </row>
     <row r="22" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -1455,10 +1456,10 @@
       <c r="C24" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="39" t="s">
+      <c r="D24" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="39"/>
+      <c r="E24" s="25"/>
       <c r="F24" s="9" t="s">
         <v>28</v>
       </c>
@@ -1468,10 +1469,10 @@
       <c r="H24" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="I24" s="39" t="s">
+      <c r="I24" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="J24" s="39"/>
+      <c r="J24" s="25"/>
       <c r="K24" s="9" t="s">
         <v>2</v>
       </c>
@@ -1492,13 +1493,13 @@
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
       <c r="K25" s="9"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
@@ -1514,19 +1515,19 @@
       <c r="W25" s="2"/>
     </row>
     <row r="26" spans="1:23" s="1" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -1541,19 +1542,19 @@
       <c r="W26" s="2"/>
     </row>
     <row r="27" spans="1:23" s="1" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -1595,10 +1596,10 @@
     <row r="29" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
-      <c r="D29" s="33" t="s">
+      <c r="D29" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="34"/>
+      <c r="E29" s="17"/>
       <c r="F29" s="13"/>
       <c r="G29" s="8" t="s">
         <v>11</v>
@@ -1623,10 +1624,10 @@
     <row r="30" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
-      <c r="D30" s="33" t="s">
+      <c r="D30" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="34"/>
+      <c r="E30" s="17"/>
       <c r="F30" s="13"/>
       <c r="G30" s="8" t="s">
         <v>11</v>
@@ -1651,10 +1652,10 @@
     <row r="31" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
-      <c r="D31" s="33" t="s">
+      <c r="D31" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="34"/>
+      <c r="E31" s="17"/>
       <c r="F31" s="13"/>
       <c r="G31" s="8" t="s">
         <v>11</v>
@@ -1679,10 +1680,10 @@
     <row r="32" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
-      <c r="D32" s="35" t="s">
+      <c r="D32" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="36"/>
+      <c r="E32" s="19"/>
       <c r="F32" s="14"/>
       <c r="G32" s="8" t="s">
         <v>15</v>
@@ -2565,7 +2566,33 @@
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:K4"/>
+    <mergeCell ref="C5:K5"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:K8"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="E21:K21"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:K11"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
     <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A26:K26"/>
+    <mergeCell ref="A27:K27"/>
+    <mergeCell ref="E22:K22"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="D32:E32"/>
@@ -2581,33 +2608,7 @@
     <mergeCell ref="A16:H16"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="A18:H18"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:K11"/>
     <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A26:K26"/>
-    <mergeCell ref="A27:K27"/>
-    <mergeCell ref="E22:K22"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:K8"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="E21:K21"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:K4"/>
-    <mergeCell ref="C5:K5"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>